<commit_message>
Cargo base de Exportaciones por aduana de Salida
El archivo se encuentra en proceso de construcción.
</commit_message>
<xml_diff>
--- a/Archivos de trabajo/Datos/Exportaciones-por-aduanas-en-Santa-Fe-segun-destino-2018-2024.xlsx
+++ b/Archivos de trabajo/Datos/Exportaciones-por-aduanas-en-Santa-Fe-segun-destino-2018-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcorvalan\Desktop\Trabajo\Paper\Paper-ITCRM.SF\Archivos de trabajo\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1853E0-C231-48C6-915C-6D756789E60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F08119-E22C-4FA8-8E6C-549858CAB72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MENSUAL" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Título</t>
   </si>
@@ -146,6 +146,9 @@
   <si>
     <t xml:space="preserve">   Arabia Saudita</t>
   </si>
+  <si>
+    <t>Paquistán</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +216,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +256,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
@@ -696,7 +705,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -806,6 +815,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="8" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -1116,6 +1128,7 @@
           <cell r="F10">
             <v>435700000</v>
           </cell>
+          <cell r="G10"/>
           <cell r="H10">
             <v>974900000</v>
           </cell>
@@ -1134,6 +1147,13 @@
           <cell r="M10">
             <v>63600000</v>
           </cell>
+          <cell r="N10"/>
+          <cell r="O10"/>
+          <cell r="P10"/>
+          <cell r="Q10"/>
+          <cell r="R10"/>
+          <cell r="S10"/>
+          <cell r="T10"/>
           <cell r="U10">
             <v>573200000</v>
           </cell>
@@ -1151,6 +1171,7 @@
           <cell r="F11">
             <v>260899999.99999997</v>
           </cell>
+          <cell r="G11"/>
           <cell r="H11">
             <v>683500000</v>
           </cell>
@@ -1163,12 +1184,19 @@
           <cell r="K11">
             <v>46500000</v>
           </cell>
+          <cell r="L11"/>
           <cell r="M11">
             <v>37800000</v>
           </cell>
+          <cell r="N11"/>
+          <cell r="O11"/>
           <cell r="P11">
             <v>40400000</v>
           </cell>
+          <cell r="Q11"/>
+          <cell r="R11"/>
+          <cell r="S11"/>
+          <cell r="T11"/>
           <cell r="U11">
             <v>432700000</v>
           </cell>
@@ -1198,15 +1226,22 @@
           <cell r="J12">
             <v>58900000</v>
           </cell>
+          <cell r="K12"/>
+          <cell r="L12"/>
           <cell r="M12">
             <v>35800000</v>
           </cell>
+          <cell r="N12"/>
+          <cell r="O12"/>
+          <cell r="P12"/>
+          <cell r="Q12"/>
           <cell r="R12">
             <v>57200000</v>
           </cell>
           <cell r="S12">
             <v>64300000</v>
           </cell>
+          <cell r="T12"/>
           <cell r="U12">
             <v>363400000</v>
           </cell>
@@ -1224,18 +1259,25 @@
           <cell r="F13">
             <v>505300000</v>
           </cell>
+          <cell r="G13"/>
           <cell r="H13">
             <v>428400000</v>
           </cell>
           <cell r="I13">
             <v>97100000</v>
           </cell>
+          <cell r="J13"/>
           <cell r="K13">
             <v>82400000</v>
           </cell>
+          <cell r="L13"/>
+          <cell r="M13"/>
+          <cell r="N13"/>
+          <cell r="O13"/>
           <cell r="P13">
             <v>86400000</v>
           </cell>
+          <cell r="Q13"/>
           <cell r="R13">
             <v>100400000</v>
           </cell>
@@ -1271,18 +1313,25 @@
           <cell r="I14">
             <v>121100000</v>
           </cell>
+          <cell r="J14"/>
+          <cell r="K14"/>
+          <cell r="L14"/>
+          <cell r="M14"/>
           <cell r="N14">
             <v>513799999.99999994</v>
           </cell>
           <cell r="O14">
             <v>339600000</v>
           </cell>
+          <cell r="P14"/>
           <cell r="Q14">
             <v>156600000</v>
           </cell>
           <cell r="R14">
             <v>144300000</v>
           </cell>
+          <cell r="S14"/>
+          <cell r="T14"/>
           <cell r="U14">
             <v>904800000</v>
           </cell>
@@ -1309,18 +1358,25 @@
           <cell r="I15">
             <v>106723973.48999999</v>
           </cell>
+          <cell r="J15"/>
+          <cell r="K15"/>
+          <cell r="L15"/>
+          <cell r="M15"/>
           <cell r="N15">
             <v>47717964.479999997</v>
           </cell>
           <cell r="O15">
             <v>218869037.96000001</v>
           </cell>
+          <cell r="P15"/>
           <cell r="Q15">
             <v>43265336.829999998</v>
           </cell>
           <cell r="R15">
             <v>89348010.709999993</v>
           </cell>
+          <cell r="S15"/>
+          <cell r="T15"/>
           <cell r="U15">
             <v>574466217.47000003</v>
           </cell>
@@ -1338,12 +1394,15 @@
           <cell r="F16">
             <v>358343403</v>
           </cell>
+          <cell r="G16"/>
           <cell r="H16">
             <v>254155904</v>
           </cell>
           <cell r="I16">
             <v>59369415</v>
           </cell>
+          <cell r="J16"/>
+          <cell r="K16"/>
           <cell r="L16">
             <v>39866151</v>
           </cell>
@@ -1356,9 +1415,13 @@
           <cell r="O16">
             <v>29339132</v>
           </cell>
+          <cell r="P16"/>
+          <cell r="Q16"/>
           <cell r="R16">
             <v>93123808</v>
           </cell>
+          <cell r="S16"/>
+          <cell r="T16"/>
           <cell r="U16">
             <v>349909153</v>
           </cell>
@@ -11468,11 +11531,11 @@
   <dimension ref="B1:AG160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C69" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A7" sqref="A7"/>
       <selection pane="topRight" activeCell="C7" sqref="C7"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D65" sqref="D65"/>
+      <selection pane="bottomRight" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11786,9 +11849,15 @@
       <c r="T9" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
+      <c r="U9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="W9" s="24" t="s">
+        <v>35</v>
+      </c>
       <c r="X9" s="24"/>
       <c r="Y9" s="24"/>
       <c r="Z9" s="24"/>
@@ -13931,31 +14000,114 @@
       <c r="C65" s="53">
         <v>1342978482</v>
       </c>
+      <c r="D65" s="53">
+        <v>5027794</v>
+      </c>
+      <c r="E65" s="53">
+        <v>166559414</v>
+      </c>
+      <c r="F65" s="53">
+        <v>64467238</v>
+      </c>
+      <c r="H65" s="53">
+        <v>88001151</v>
+      </c>
+      <c r="I65" s="53">
+        <v>86712557</v>
+      </c>
+      <c r="J65" s="53">
+        <v>40141913</v>
+      </c>
+      <c r="Q65" s="53">
+        <v>84715416</v>
+      </c>
+      <c r="R65" s="53">
+        <v>22488556</v>
+      </c>
+      <c r="U65" s="53">
+        <v>66851550</v>
+      </c>
+      <c r="V65" s="53">
+        <v>51007233</v>
+      </c>
+      <c r="AG65" s="53">
+        <v>667005660</v>
+      </c>
     </row>
     <row r="66" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B66" s="26">
         <v>2023.02</v>
       </c>
+      <c r="C66" s="53">
+        <v>2793133144</v>
+      </c>
+      <c r="E66" s="53">
+        <v>352712414</v>
+      </c>
+      <c r="F66" s="53">
+        <v>131622059</v>
+      </c>
+      <c r="G66" s="53">
+        <v>85116912</v>
+      </c>
+      <c r="H66" s="53">
+        <v>205291313</v>
+      </c>
+      <c r="I66" s="53">
+        <v>115565370</v>
+      </c>
+      <c r="J66" s="53">
+        <v>93175050</v>
+      </c>
+      <c r="O66" s="53">
+        <v>56969089</v>
+      </c>
+      <c r="Q66" s="53">
+        <v>221776966</v>
+      </c>
+      <c r="AG66" s="53">
+        <v>1530903971</v>
+      </c>
     </row>
     <row r="67" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B67" s="26">
         <v>2023.03</v>
       </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="29"/>
-      <c r="F67" s="29"/>
-      <c r="G67" s="29"/>
-      <c r="H67" s="29"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="29"/>
+      <c r="C67" s="53">
+        <v>4395069701.9099998</v>
+      </c>
+      <c r="D67" s="53">
+        <v>197988466.50999999</v>
+      </c>
+      <c r="E67" s="53">
+        <v>480466625.70999998</v>
+      </c>
+      <c r="F67" s="53">
+        <v>184256982.72</v>
+      </c>
+      <c r="G67" s="53">
+        <v>160111703.25999999</v>
+      </c>
+      <c r="H67" s="53">
+        <v>286801982.47000003</v>
+      </c>
+      <c r="I67" s="53">
+        <v>228327643.33000001</v>
+      </c>
+      <c r="J67" s="53">
+        <v>169952592.19999999</v>
+      </c>
       <c r="K67" s="29"/>
       <c r="L67" s="29"/>
       <c r="M67" s="29"/>
       <c r="N67" s="29"/>
-      <c r="O67" s="29"/>
+      <c r="O67" s="53">
+        <v>98424409.299999997</v>
+      </c>
       <c r="P67" s="29"/>
-      <c r="Q67" s="29"/>
+      <c r="Q67" s="53">
+        <v>369476180.57999998</v>
+      </c>
       <c r="R67" s="29"/>
       <c r="S67" s="29"/>
       <c r="T67" s="29"/>
@@ -13971,30 +14123,54 @@
       <c r="AD67" s="29"/>
       <c r="AE67" s="29"/>
       <c r="AF67" s="30"/>
-      <c r="AG67" s="31"/>
+      <c r="AG67" s="53">
+        <v>2219263115.8299999</v>
+      </c>
     </row>
     <row r="68" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B68" s="26">
         <v>2023.04</v>
       </c>
-      <c r="C68" s="32"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="29"/>
-      <c r="F68" s="29"/>
-      <c r="G68" s="29"/>
-      <c r="H68" s="29"/>
-      <c r="I68" s="29"/>
-      <c r="J68" s="29"/>
+      <c r="C68" s="53">
+        <v>6336450965.9099998</v>
+      </c>
+      <c r="D68" s="53">
+        <v>235005827.50999999</v>
+      </c>
+      <c r="E68" s="53">
+        <v>691846815.71000004</v>
+      </c>
+      <c r="F68" s="53">
+        <v>337500078.72000003</v>
+      </c>
+      <c r="G68" s="53">
+        <v>288941924.25999999</v>
+      </c>
+      <c r="H68" s="53">
+        <v>336342079.47000003</v>
+      </c>
+      <c r="I68" s="53">
+        <v>316509161.32999998</v>
+      </c>
+      <c r="J68" s="53">
+        <v>224318655.19999999</v>
+      </c>
       <c r="K68" s="29"/>
       <c r="L68" s="29"/>
       <c r="M68" s="29"/>
       <c r="N68" s="29"/>
-      <c r="O68" s="29"/>
+      <c r="O68" s="53">
+        <v>162910132.30000001</v>
+      </c>
       <c r="P68" s="29"/>
-      <c r="Q68" s="29"/>
+      <c r="Q68" s="53">
+        <v>461422251.57999998</v>
+      </c>
       <c r="R68" s="29"/>
       <c r="S68" s="29"/>
-      <c r="T68" s="29"/>
+      <c r="T68" s="53">
+        <v>102016903.98999999</v>
+      </c>
       <c r="U68" s="29"/>
       <c r="V68" s="29"/>
       <c r="W68" s="29"/>
@@ -14007,30 +14183,54 @@
       <c r="AD68" s="29"/>
       <c r="AE68" s="29"/>
       <c r="AF68" s="30"/>
-      <c r="AG68" s="31"/>
+      <c r="AG68" s="53">
+        <v>3179637135.8400002</v>
+      </c>
     </row>
     <row r="69" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B69" s="26">
         <v>2023.05</v>
       </c>
-      <c r="C69" s="32"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="29"/>
-      <c r="F69" s="29"/>
-      <c r="G69" s="29"/>
-      <c r="H69" s="29"/>
-      <c r="I69" s="29"/>
-      <c r="J69" s="29"/>
+      <c r="C69" s="53">
+        <v>8380565475.9099998</v>
+      </c>
+      <c r="D69" s="53">
+        <v>388959171.50999999</v>
+      </c>
+      <c r="E69" s="53">
+        <v>985379574.71000004</v>
+      </c>
+      <c r="F69" s="53">
+        <v>503482172.72000003</v>
+      </c>
+      <c r="G69" s="53">
+        <v>344123112.25999999</v>
+      </c>
+      <c r="H69" s="53">
+        <v>473974773.47000003</v>
+      </c>
+      <c r="I69" s="53">
+        <v>395144607.32999998</v>
+      </c>
+      <c r="J69" s="53">
+        <v>269282197.19999999</v>
+      </c>
       <c r="K69" s="29"/>
       <c r="L69" s="29"/>
       <c r="M69" s="29"/>
       <c r="N69" s="29"/>
       <c r="O69" s="29"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="29"/>
+      <c r="P69" s="53">
+        <v>196059447.41</v>
+      </c>
+      <c r="Q69" s="53">
+        <v>555243708.58000004</v>
+      </c>
       <c r="R69" s="29"/>
       <c r="S69" s="29"/>
-      <c r="T69" s="29"/>
+      <c r="T69" s="53">
+        <v>136727641.99000001</v>
+      </c>
       <c r="U69" s="29"/>
       <c r="V69" s="29"/>
       <c r="W69" s="29"/>
@@ -14043,30 +14243,54 @@
       <c r="AD69" s="29"/>
       <c r="AE69" s="29"/>
       <c r="AF69" s="30"/>
-      <c r="AG69" s="31"/>
+      <c r="AG69" s="53">
+        <v>4132189068.73</v>
+      </c>
     </row>
     <row r="70" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B70" s="26">
         <v>2023.06</v>
       </c>
-      <c r="C70" s="32"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="29"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
-      <c r="H70" s="29"/>
-      <c r="I70" s="29"/>
-      <c r="J70" s="29"/>
+      <c r="C70" s="53">
+        <v>10246888189.91</v>
+      </c>
+      <c r="D70" s="53">
+        <v>454192299.50999999</v>
+      </c>
+      <c r="E70" s="53">
+        <v>1186425147.71</v>
+      </c>
+      <c r="F70" s="53">
+        <v>730208897.72000003</v>
+      </c>
+      <c r="G70" s="53">
+        <v>423208825.25999999</v>
+      </c>
+      <c r="H70" s="53">
+        <v>514036728.47000003</v>
+      </c>
+      <c r="I70" s="53">
+        <v>438290386.32999998</v>
+      </c>
+      <c r="J70" s="53">
+        <v>312655675.19999999</v>
+      </c>
       <c r="K70" s="29"/>
       <c r="L70" s="29"/>
       <c r="M70" s="29"/>
       <c r="N70" s="29"/>
       <c r="O70" s="29"/>
-      <c r="P70" s="29"/>
-      <c r="Q70" s="29"/>
+      <c r="P70" s="53">
+        <v>284765964.41000003</v>
+      </c>
+      <c r="Q70" s="53">
+        <v>655030345.58000004</v>
+      </c>
       <c r="R70" s="29"/>
       <c r="S70" s="29"/>
-      <c r="T70" s="29"/>
+      <c r="T70" s="53">
+        <v>158573252.99000001</v>
+      </c>
       <c r="U70" s="29"/>
       <c r="V70" s="29"/>
       <c r="W70" s="29"/>
@@ -14079,30 +14303,54 @@
       <c r="AD70" s="29"/>
       <c r="AE70" s="29"/>
       <c r="AF70" s="30"/>
-      <c r="AG70" s="31"/>
+      <c r="AG70" s="53">
+        <v>5089500666.7299995</v>
+      </c>
     </row>
     <row r="71" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B71" s="26">
         <v>2023.07</v>
       </c>
-      <c r="C71" s="32"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="29"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
-      <c r="H71" s="29"/>
-      <c r="I71" s="29"/>
-      <c r="J71" s="29"/>
+      <c r="C71" s="53">
+        <v>12006219282.91</v>
+      </c>
+      <c r="D71" s="53">
+        <v>524888116.50999999</v>
+      </c>
+      <c r="E71" s="53">
+        <v>1319005364.71</v>
+      </c>
+      <c r="F71" s="53">
+        <v>937006063.72000003</v>
+      </c>
+      <c r="G71" s="53">
+        <v>483369337.25999999</v>
+      </c>
+      <c r="H71" s="53">
+        <v>530123193.47000003</v>
+      </c>
+      <c r="I71" s="53">
+        <v>541313434.33000004</v>
+      </c>
+      <c r="J71" s="53">
+        <v>324145870.19999999</v>
+      </c>
       <c r="K71" s="29"/>
       <c r="L71" s="29"/>
       <c r="M71" s="29"/>
       <c r="N71" s="29"/>
       <c r="O71" s="29"/>
-      <c r="P71" s="29"/>
-      <c r="Q71" s="29"/>
+      <c r="P71" s="53">
+        <v>394113423.41000003</v>
+      </c>
+      <c r="Q71" s="53">
+        <v>744419992.58000004</v>
+      </c>
       <c r="R71" s="29"/>
       <c r="S71" s="29"/>
-      <c r="T71" s="29"/>
+      <c r="T71" s="53">
+        <v>231219097.99000001</v>
+      </c>
       <c r="U71" s="29"/>
       <c r="V71" s="29"/>
       <c r="W71" s="29"/>
@@ -14115,30 +14363,54 @@
       <c r="AD71" s="29"/>
       <c r="AE71" s="29"/>
       <c r="AF71" s="30"/>
-      <c r="AG71" s="31"/>
+      <c r="AG71" s="53">
+        <v>5976615388.7299995</v>
+      </c>
     </row>
     <row r="72" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B72" s="26">
         <v>2023.08</v>
       </c>
-      <c r="C72" s="32"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="29"/>
-      <c r="F72" s="29"/>
-      <c r="G72" s="29"/>
-      <c r="H72" s="29"/>
-      <c r="I72" s="29"/>
-      <c r="J72" s="29"/>
+      <c r="C72" s="53">
+        <v>13876539701.91</v>
+      </c>
+      <c r="D72" s="53">
+        <v>575018544.50999999</v>
+      </c>
+      <c r="E72" s="53">
+        <v>1366409003.71</v>
+      </c>
+      <c r="F72" s="53">
+        <v>1127640884.72</v>
+      </c>
+      <c r="G72" s="53">
+        <v>610100116.25999999</v>
+      </c>
+      <c r="H72" s="53">
+        <v>597130066.47000003</v>
+      </c>
+      <c r="I72" s="53">
+        <v>604173946.33000004</v>
+      </c>
+      <c r="J72" s="53">
+        <v>361172415.19999999</v>
+      </c>
       <c r="K72" s="29"/>
       <c r="L72" s="29"/>
       <c r="M72" s="29"/>
       <c r="N72" s="29"/>
       <c r="O72" s="29"/>
-      <c r="P72" s="29"/>
-      <c r="Q72" s="29"/>
+      <c r="P72" s="53">
+        <v>443030842.41000003</v>
+      </c>
+      <c r="Q72" s="53">
+        <v>811449355.58000004</v>
+      </c>
       <c r="R72" s="29"/>
       <c r="S72" s="29"/>
-      <c r="T72" s="29"/>
+      <c r="T72" s="53">
+        <v>287884489.99000001</v>
+      </c>
       <c r="U72" s="29"/>
       <c r="V72" s="29"/>
       <c r="W72" s="29"/>
@@ -14151,7 +14423,9 @@
       <c r="AD72" s="29"/>
       <c r="AE72" s="29"/>
       <c r="AF72" s="30"/>
-      <c r="AG72" s="31"/>
+      <c r="AG72" s="53">
+        <v>7092530036.7299995</v>
+      </c>
     </row>
     <row r="73" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B73" s="26">
@@ -14341,8 +14615,12 @@
       <c r="T77" s="53">
         <v>57312966</v>
       </c>
-      <c r="U77" s="29"/>
-      <c r="V77" s="29"/>
+      <c r="U77" s="55">
+        <v>130080000</v>
+      </c>
+      <c r="V77" s="55">
+        <v>105230070</v>
+      </c>
       <c r="W77" s="29"/>
       <c r="X77" s="29"/>
       <c r="Y77" s="29"/>
@@ -14373,7 +14651,9 @@
       <c r="F78" s="53">
         <v>262364409</v>
       </c>
-      <c r="G78" s="29"/>
+      <c r="G78" s="55">
+        <v>87477604</v>
+      </c>
       <c r="H78" s="53">
         <v>160810826</v>
       </c>
@@ -14387,7 +14667,9 @@
       <c r="L78" s="29"/>
       <c r="M78" s="29"/>
       <c r="N78" s="29"/>
-      <c r="O78" s="29"/>
+      <c r="O78" s="55">
+        <v>111918936</v>
+      </c>
       <c r="P78" s="29"/>
       <c r="Q78" s="53">
         <v>242562181</v>
@@ -14403,7 +14685,9 @@
       </c>
       <c r="U78" s="29"/>
       <c r="V78" s="29"/>
-      <c r="W78" s="29"/>
+      <c r="W78" s="55">
+        <v>225169108</v>
+      </c>
       <c r="X78" s="29"/>
       <c r="Y78" s="29"/>
       <c r="Z78" s="29"/>
@@ -14433,7 +14717,9 @@
       <c r="F79" s="53">
         <v>502781721</v>
       </c>
-      <c r="G79" s="29"/>
+      <c r="G79" s="55">
+        <v>134426087</v>
+      </c>
       <c r="H79" s="53">
         <v>243246205</v>
       </c>
@@ -14447,7 +14733,9 @@
       <c r="L79" s="29"/>
       <c r="M79" s="29"/>
       <c r="N79" s="29"/>
-      <c r="O79" s="29"/>
+      <c r="O79" s="55">
+        <v>176176161</v>
+      </c>
       <c r="P79" s="29"/>
       <c r="Q79" s="53">
         <v>396712142</v>
@@ -14493,7 +14781,9 @@
       <c r="F80" s="53">
         <v>766304219</v>
       </c>
-      <c r="G80" s="29"/>
+      <c r="G80" s="55">
+        <v>181252406</v>
+      </c>
       <c r="H80" s="53">
         <v>259729898</v>
       </c>
@@ -14507,7 +14797,9 @@
       <c r="L80" s="29"/>
       <c r="M80" s="29"/>
       <c r="N80" s="29"/>
-      <c r="O80" s="29"/>
+      <c r="O80" s="55">
+        <v>224774558</v>
+      </c>
       <c r="P80" s="29"/>
       <c r="Q80" s="53">
         <v>500072631</v>
@@ -14553,7 +14845,9 @@
       <c r="F81" s="53">
         <v>980478984</v>
       </c>
-      <c r="G81" s="29"/>
+      <c r="G81" s="55">
+        <v>229049519</v>
+      </c>
       <c r="H81" s="53">
         <v>335689367</v>
       </c>
@@ -14613,7 +14907,9 @@
       <c r="F82" s="53">
         <v>1158814518.45</v>
       </c>
-      <c r="G82" s="29"/>
+      <c r="G82" s="55">
+        <v>265572337</v>
+      </c>
       <c r="H82" s="53">
         <v>431051108.51999998</v>
       </c>
@@ -14661,24 +14957,46 @@
       <c r="B83" s="26">
         <v>2024.07</v>
       </c>
-      <c r="C83" s="32"/>
-      <c r="D83" s="28"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
+      <c r="C83" s="53">
+        <v>15761004674</v>
+      </c>
+      <c r="D83" s="53">
+        <v>504642603</v>
+      </c>
+      <c r="E83" s="53">
+        <v>1506785960</v>
+      </c>
+      <c r="F83" s="53">
+        <v>1332911671</v>
+      </c>
+      <c r="G83" s="53">
+        <v>265572337</v>
+      </c>
+      <c r="H83" s="53">
+        <v>519350972</v>
+      </c>
+      <c r="I83" s="53">
+        <v>586159898</v>
+      </c>
+      <c r="J83" s="53">
+        <v>628218916</v>
+      </c>
       <c r="K83" s="29"/>
       <c r="L83" s="29"/>
       <c r="M83" s="29"/>
       <c r="N83" s="29"/>
       <c r="O83" s="29"/>
-      <c r="P83" s="29"/>
-      <c r="Q83" s="29"/>
+      <c r="P83" s="53">
+        <v>925725266</v>
+      </c>
+      <c r="Q83" s="53">
+        <v>797192600</v>
+      </c>
       <c r="R83" s="29"/>
       <c r="S83" s="29"/>
-      <c r="T83" s="29"/>
+      <c r="T83" s="53">
+        <v>517726052</v>
+      </c>
       <c r="U83" s="29"/>
       <c r="V83" s="29"/>
       <c r="W83" s="29"/>
@@ -14691,30 +15009,54 @@
       <c r="AD83" s="29"/>
       <c r="AE83" s="29"/>
       <c r="AF83" s="30"/>
-      <c r="AG83" s="31"/>
+      <c r="AG83" s="53">
+        <v>8176718399</v>
+      </c>
     </row>
     <row r="84" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B84" s="26">
         <v>2024.08</v>
       </c>
-      <c r="C84" s="32"/>
-      <c r="D84" s="28"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="29"/>
-      <c r="G84" s="29"/>
-      <c r="H84" s="29"/>
-      <c r="I84" s="29"/>
-      <c r="J84" s="29"/>
+      <c r="C84" s="53">
+        <v>17706016667</v>
+      </c>
+      <c r="D84" s="53">
+        <v>548546991</v>
+      </c>
+      <c r="E84" s="53">
+        <v>1694006851</v>
+      </c>
+      <c r="F84" s="53">
+        <v>1537588748</v>
+      </c>
+      <c r="G84" s="53">
+        <v>283499280</v>
+      </c>
+      <c r="H84" s="53">
+        <v>569164653</v>
+      </c>
+      <c r="I84" s="53">
+        <v>647988480</v>
+      </c>
+      <c r="J84" s="53">
+        <v>692589872</v>
+      </c>
       <c r="K84" s="29"/>
       <c r="L84" s="29"/>
       <c r="M84" s="29"/>
       <c r="N84" s="29"/>
       <c r="O84" s="29"/>
-      <c r="P84" s="29"/>
-      <c r="Q84" s="29"/>
+      <c r="P84" s="53">
+        <v>1020778355</v>
+      </c>
+      <c r="Q84" s="53">
+        <v>902768655</v>
+      </c>
       <c r="R84" s="29"/>
       <c r="S84" s="29"/>
-      <c r="T84" s="29"/>
+      <c r="T84" s="53">
+        <v>602362186</v>
+      </c>
       <c r="U84" s="29"/>
       <c r="V84" s="29"/>
       <c r="W84" s="29"/>
@@ -14727,7 +15069,9 @@
       <c r="AD84" s="29"/>
       <c r="AE84" s="29"/>
       <c r="AF84" s="30"/>
-      <c r="AG84" s="31"/>
+      <c r="AG84" s="53">
+        <v>9206722596</v>
+      </c>
     </row>
     <row r="85" spans="2:33" x14ac:dyDescent="0.25">
       <c r="B85" s="26">

</xml_diff>